<commit_message>
Procedure to load rates
</commit_message>
<xml_diff>
--- a/data/auspost-rates-data.xlsx
+++ b/data/auspost-rates-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AusPost data" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4792" uniqueCount="1652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4789" uniqueCount="1650">
   <si>
     <t xml:space="preserve">Australia Post data</t>
   </si>
@@ -4977,12 +4977,6 @@
   </si>
   <si>
     <t xml:space="preserve">Zones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone 4: USA and Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone 6: UK and Ireland</t>
   </si>
 </sst>
 </file>
@@ -4999,6 +4993,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -5020,12 +5015,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -5192,7 +5189,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5221,7 +5218,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -19873,7 +19870,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -19892,7 +19889,7 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -20581,7 +20578,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -20596,11 +20593,11 @@
   </sheetPr>
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.8"/>
   </cols>
@@ -23046,7 +23043,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -23065,10 +23062,10 @@
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="11.52"/>
@@ -23578,7 +23575,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A24,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B24" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F24</f>
@@ -23600,7 +23597,7 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A25,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B25" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F25</f>
@@ -23622,7 +23619,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A26,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B26" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F26</f>
@@ -23644,7 +23641,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A27,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B27" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F27</f>
@@ -23666,7 +23663,7 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A28,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B28" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F28</f>
@@ -23688,7 +23685,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A29,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B29" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F29</f>
@@ -23842,7 +23839,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A36,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B36" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F36</f>
@@ -23864,7 +23861,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A37,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B37" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F37</f>
@@ -23886,7 +23883,7 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A38,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B38" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F38</f>
@@ -23908,7 +23905,7 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A39,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B39" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F39</f>
@@ -23930,7 +23927,7 @@
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A40,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B40" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F40</f>
@@ -23952,7 +23949,7 @@
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 1'!A41,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B41" s="0" t="str">
         <f aca="false">'Rate definitions 1'!F41</f>
@@ -24370,7 +24367,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -24383,13 +24380,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.19"/>
   </cols>
@@ -25306,33 +25303,31 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="str">
-        <f aca="false">A22</f>
-        <v>Zone 2</v>
+      <c r="A23" s="0" t="s">
+        <v>1610</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C23" s="0" t="n">
-        <f aca="false">D22</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>1631</v>
+        <v>1646</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>1641</v>
+        <v>1648</v>
       </c>
       <c r="G23" s="0" t="n">
         <f aca="false">MATCH(D23,'Rate calcs'!$A$24:$A$30,0)+IF(B23="Express",12,0)</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H23" s="0" t="n">
         <f aca="false">MATCH(A23,'Rate calcs'!$B$23:$K$23,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I23" s="4" t="n">
         <f aca="false">IF(E23="Yes",(D23*'Rate calcs'!$C$8-100)/100*IF(A23="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
@@ -25340,25 +25335,27 @@
       </c>
       <c r="J23" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G23,H23)</f>
-        <v>47.9</v>
+        <v>34</v>
       </c>
       <c r="K23" s="0" t="n">
         <f aca="false">I23+J23</f>
-        <v>47.9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>1610</v>
+      <c r="A24" s="0" t="str">
+        <f aca="false">A23</f>
+        <v>Zone 3</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>0</v>
+        <f aca="false">D23</f>
+        <v>0.25</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>1646</v>
@@ -25368,7 +25365,7 @@
       </c>
       <c r="G24" s="0" t="n">
         <f aca="false">MATCH(D24,'Rate calcs'!$A$24:$A$30,0)+IF(B24="Express",12,0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H24" s="0" t="n">
         <f aca="false">MATCH(A24,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25376,15 +25373,15 @@
       </c>
       <c r="I24" s="4" t="n">
         <f aca="false">IF(E24="Yes",(D24*'Rate calcs'!$C$8-100)/100*IF(A24="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J24" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G24,H24)</f>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K24" s="0" t="n">
         <f aca="false">I24+J24</f>
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25397,10 +25394,10 @@
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">D24</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>1646</v>
@@ -25410,7 +25407,7 @@
       </c>
       <c r="G25" s="0" t="n">
         <f aca="false">MATCH(D25,'Rate calcs'!$A$24:$A$30,0)+IF(B25="Express",12,0)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H25" s="0" t="n">
         <f aca="false">MATCH(A25,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25418,15 +25415,15 @@
       </c>
       <c r="I25" s="4" t="n">
         <f aca="false">IF(E25="Yes",(D25*'Rate calcs'!$C$8-100)/100*IF(A25="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J25" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G25,H25)</f>
-        <v>37</v>
+        <v>48.7</v>
       </c>
       <c r="K25" s="0" t="n">
         <f aca="false">I25+J25</f>
-        <v>41</v>
+        <v>60.7</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25439,10 +25436,10 @@
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">D25</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>1646</v>
@@ -25452,7 +25449,7 @@
       </c>
       <c r="G26" s="0" t="n">
         <f aca="false">MATCH(D26,'Rate calcs'!$A$24:$A$30,0)+IF(B26="Express",12,0)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H26" s="0" t="n">
         <f aca="false">MATCH(A26,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25460,15 +25457,15 @@
       </c>
       <c r="I26" s="4" t="n">
         <f aca="false">IF(E26="Yes",(D26*'Rate calcs'!$C$8-100)/100*IF(A26="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J26" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G26,H26)</f>
-        <v>48.7</v>
+        <v>60.4</v>
       </c>
       <c r="K26" s="0" t="n">
         <f aca="false">I26+J26</f>
-        <v>60.7</v>
+        <v>80.4</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25481,10 +25478,10 @@
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">D26</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>1646</v>
@@ -25494,7 +25491,7 @@
       </c>
       <c r="G27" s="0" t="n">
         <f aca="false">MATCH(D27,'Rate calcs'!$A$24:$A$30,0)+IF(B27="Express",12,0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H27" s="0" t="n">
         <f aca="false">MATCH(A27,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25502,15 +25499,15 @@
       </c>
       <c r="I27" s="4" t="n">
         <f aca="false">IF(E27="Yes",(D27*'Rate calcs'!$C$8-100)/100*IF(A27="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J27" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G27,H27)</f>
-        <v>60.4</v>
+        <v>72.1</v>
       </c>
       <c r="K27" s="0" t="n">
         <f aca="false">I27+J27</f>
-        <v>80.4</v>
+        <v>100.1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25523,10 +25520,10 @@
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">D27</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>1646</v>
@@ -25536,7 +25533,7 @@
       </c>
       <c r="G28" s="0" t="n">
         <f aca="false">MATCH(D28,'Rate calcs'!$A$24:$A$30,0)+IF(B28="Express",12,0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H28" s="0" t="n">
         <f aca="false">MATCH(A28,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25544,15 +25541,15 @@
       </c>
       <c r="I28" s="4" t="n">
         <f aca="false">IF(E28="Yes",(D28*'Rate calcs'!$C$8-100)/100*IF(A28="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="J28" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G28,H28)</f>
-        <v>72.1</v>
+        <v>80.8</v>
       </c>
       <c r="K28" s="0" t="n">
         <f aca="false">I28+J28</f>
-        <v>100.1</v>
+        <v>124.8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25565,10 +25562,10 @@
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">D28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>1646</v>
@@ -25578,7 +25575,7 @@
       </c>
       <c r="G29" s="0" t="n">
         <f aca="false">MATCH(D29,'Rate calcs'!$A$24:$A$30,0)+IF(B29="Express",12,0)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H29" s="0" t="n">
         <f aca="false">MATCH(A29,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25586,31 +25583,29 @@
       </c>
       <c r="I29" s="4" t="n">
         <f aca="false">IF(E29="Yes",(D29*'Rate calcs'!$C$8-100)/100*IF(A29="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="J29" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G29,H29)</f>
-        <v>80.8</v>
+        <v>98.2</v>
       </c>
       <c r="K29" s="0" t="n">
         <f aca="false">I29+J29</f>
-        <v>124.8</v>
+        <v>174.2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="str">
-        <f aca="false">A29</f>
-        <v>Zone 3</v>
+      <c r="A30" s="0" t="s">
+        <v>1611</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C30" s="0" t="n">
-        <f aca="false">D29</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>1646</v>
@@ -25620,37 +25615,39 @@
       </c>
       <c r="G30" s="0" t="n">
         <f aca="false">MATCH(D30,'Rate calcs'!$A$24:$A$30,0)+IF(B30="Express",12,0)</f>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H30" s="0" t="n">
         <f aca="false">MATCH(A30,'Rate calcs'!$B$23:$K$23,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I30" s="4" t="n">
         <f aca="false">IF(E30="Yes",(D30*'Rate calcs'!$C$8-100)/100*IF(A30="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="J30" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G30,H30)</f>
-        <v>98.2</v>
+        <v>36</v>
       </c>
       <c r="K30" s="0" t="n">
         <f aca="false">I30+J30</f>
-        <v>174.2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>1611</v>
+      <c r="A31" s="0" t="str">
+        <f aca="false">A30</f>
+        <v>Zone 4</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>0</v>
+        <f aca="false">D30</f>
+        <v>0.25</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>1646</v>
@@ -25660,7 +25657,7 @@
       </c>
       <c r="G31" s="0" t="n">
         <f aca="false">MATCH(D31,'Rate calcs'!$A$24:$A$30,0)+IF(B31="Express",12,0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H31" s="0" t="n">
         <f aca="false">MATCH(A31,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25668,15 +25665,15 @@
       </c>
       <c r="I31" s="4" t="n">
         <f aca="false">IF(E31="Yes",(D31*'Rate calcs'!$C$8-100)/100*IF(A31="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J31" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G31,H31)</f>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K31" s="0" t="n">
         <f aca="false">I31+J31</f>
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25689,10 +25686,10 @@
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">D31</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>1646</v>
@@ -25702,7 +25699,7 @@
       </c>
       <c r="G32" s="0" t="n">
         <f aca="false">MATCH(D32,'Rate calcs'!$A$24:$A$30,0)+IF(B32="Express",12,0)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H32" s="0" t="n">
         <f aca="false">MATCH(A32,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25710,15 +25707,15 @@
       </c>
       <c r="I32" s="4" t="n">
         <f aca="false">IF(E32="Yes",(D32*'Rate calcs'!$C$8-100)/100*IF(A32="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J32" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G32,H32)</f>
-        <v>39</v>
+        <v>51.9</v>
       </c>
       <c r="K32" s="0" t="n">
         <f aca="false">I32+J32</f>
-        <v>43</v>
+        <v>63.9</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25731,10 +25728,10 @@
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">D32</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>1646</v>
@@ -25744,7 +25741,7 @@
       </c>
       <c r="G33" s="0" t="n">
         <f aca="false">MATCH(D33,'Rate calcs'!$A$24:$A$30,0)+IF(B33="Express",12,0)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H33" s="0" t="n">
         <f aca="false">MATCH(A33,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25752,15 +25749,15 @@
       </c>
       <c r="I33" s="4" t="n">
         <f aca="false">IF(E33="Yes",(D33*'Rate calcs'!$C$8-100)/100*IF(A33="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J33" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G33,H33)</f>
-        <v>51.9</v>
+        <v>64.8</v>
       </c>
       <c r="K33" s="0" t="n">
         <f aca="false">I33+J33</f>
-        <v>63.9</v>
+        <v>84.8</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25773,10 +25770,10 @@
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">D33</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>1646</v>
@@ -25786,7 +25783,7 @@
       </c>
       <c r="G34" s="0" t="n">
         <f aca="false">MATCH(D34,'Rate calcs'!$A$24:$A$30,0)+IF(B34="Express",12,0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H34" s="0" t="n">
         <f aca="false">MATCH(A34,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25794,15 +25791,15 @@
       </c>
       <c r="I34" s="4" t="n">
         <f aca="false">IF(E34="Yes",(D34*'Rate calcs'!$C$8-100)/100*IF(A34="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J34" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G34,H34)</f>
-        <v>64.8</v>
+        <v>77.7</v>
       </c>
       <c r="K34" s="0" t="n">
         <f aca="false">I34+J34</f>
-        <v>84.8</v>
+        <v>105.7</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25815,10 +25812,10 @@
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">D34</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>1646</v>
@@ -25828,7 +25825,7 @@
       </c>
       <c r="G35" s="0" t="n">
         <f aca="false">MATCH(D35,'Rate calcs'!$A$24:$A$30,0)+IF(B35="Express",12,0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H35" s="0" t="n">
         <f aca="false">MATCH(A35,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25836,15 +25833,15 @@
       </c>
       <c r="I35" s="4" t="n">
         <f aca="false">IF(E35="Yes",(D35*'Rate calcs'!$C$8-100)/100*IF(A35="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="J35" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G35,H35)</f>
-        <v>77.7</v>
+        <v>86.5</v>
       </c>
       <c r="K35" s="0" t="n">
         <f aca="false">I35+J35</f>
-        <v>105.7</v>
+        <v>130.5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25857,10 +25854,10 @@
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">D35</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>1646</v>
@@ -25870,7 +25867,7 @@
       </c>
       <c r="G36" s="0" t="n">
         <f aca="false">MATCH(D36,'Rate calcs'!$A$24:$A$30,0)+IF(B36="Express",12,0)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H36" s="0" t="n">
         <f aca="false">MATCH(A36,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25878,31 +25875,29 @@
       </c>
       <c r="I36" s="4" t="n">
         <f aca="false">IF(E36="Yes",(D36*'Rate calcs'!$C$8-100)/100*IF(A36="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="J36" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G36,H36)</f>
-        <v>86.5</v>
+        <v>104.1</v>
       </c>
       <c r="K36" s="0" t="n">
         <f aca="false">I36+J36</f>
-        <v>130.5</v>
+        <v>180.1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="str">
-        <f aca="false">A36</f>
-        <v>Zone 4</v>
+      <c r="A37" s="0" t="s">
+        <v>1612</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C37" s="0" t="n">
-        <f aca="false">D36</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>1646</v>
@@ -25912,37 +25907,39 @@
       </c>
       <c r="G37" s="0" t="n">
         <f aca="false">MATCH(D37,'Rate calcs'!$A$24:$A$30,0)+IF(B37="Express",12,0)</f>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H37" s="0" t="n">
         <f aca="false">MATCH(A37,'Rate calcs'!$B$23:$K$23,0)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I37" s="4" t="n">
         <f aca="false">IF(E37="Yes",(D37*'Rate calcs'!$C$8-100)/100*IF(A37="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="J37" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G37,H37)</f>
-        <v>104.1</v>
+        <v>34.5</v>
       </c>
       <c r="K37" s="0" t="n">
         <f aca="false">I37+J37</f>
-        <v>180.1</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>1612</v>
+      <c r="A38" s="0" t="str">
+        <f aca="false">A37</f>
+        <v>Zone 5</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>0</v>
+        <f aca="false">D37</f>
+        <v>0.25</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>1646</v>
@@ -25952,7 +25949,7 @@
       </c>
       <c r="G38" s="0" t="n">
         <f aca="false">MATCH(D38,'Rate calcs'!$A$24:$A$30,0)+IF(B38="Express",12,0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H38" s="0" t="n">
         <f aca="false">MATCH(A38,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -25960,15 +25957,15 @@
       </c>
       <c r="I38" s="4" t="n">
         <f aca="false">IF(E38="Yes",(D38*'Rate calcs'!$C$8-100)/100*IF(A38="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J38" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G38,H38)</f>
-        <v>34.5</v>
+        <v>37.5</v>
       </c>
       <c r="K38" s="0" t="n">
         <f aca="false">I38+J38</f>
-        <v>34.5</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25981,10 +25978,10 @@
       </c>
       <c r="C39" s="0" t="n">
         <f aca="false">D38</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>1646</v>
@@ -25994,7 +25991,7 @@
       </c>
       <c r="G39" s="0" t="n">
         <f aca="false">MATCH(D39,'Rate calcs'!$A$24:$A$30,0)+IF(B39="Express",12,0)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H39" s="0" t="n">
         <f aca="false">MATCH(A39,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26002,15 +25999,15 @@
       </c>
       <c r="I39" s="4" t="n">
         <f aca="false">IF(E39="Yes",(D39*'Rate calcs'!$C$8-100)/100*IF(A39="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J39" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G39,H39)</f>
-        <v>37.5</v>
+        <v>49.2</v>
       </c>
       <c r="K39" s="0" t="n">
         <f aca="false">I39+J39</f>
-        <v>41.5</v>
+        <v>61.2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26023,10 +26020,10 @@
       </c>
       <c r="C40" s="0" t="n">
         <f aca="false">D39</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>1646</v>
@@ -26036,7 +26033,7 @@
       </c>
       <c r="G40" s="0" t="n">
         <f aca="false">MATCH(D40,'Rate calcs'!$A$24:$A$30,0)+IF(B40="Express",12,0)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H40" s="0" t="n">
         <f aca="false">MATCH(A40,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26044,15 +26041,15 @@
       </c>
       <c r="I40" s="4" t="n">
         <f aca="false">IF(E40="Yes",(D40*'Rate calcs'!$C$8-100)/100*IF(A40="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J40" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G40,H40)</f>
-        <v>49.2</v>
+        <v>60.9</v>
       </c>
       <c r="K40" s="0" t="n">
         <f aca="false">I40+J40</f>
-        <v>61.2</v>
+        <v>80.9</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26065,10 +26062,10 @@
       </c>
       <c r="C41" s="0" t="n">
         <f aca="false">D40</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>1646</v>
@@ -26078,7 +26075,7 @@
       </c>
       <c r="G41" s="0" t="n">
         <f aca="false">MATCH(D41,'Rate calcs'!$A$24:$A$30,0)+IF(B41="Express",12,0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H41" s="0" t="n">
         <f aca="false">MATCH(A41,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26086,15 +26083,15 @@
       </c>
       <c r="I41" s="4" t="n">
         <f aca="false">IF(E41="Yes",(D41*'Rate calcs'!$C$8-100)/100*IF(A41="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J41" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G41,H41)</f>
-        <v>60.9</v>
+        <v>72.6</v>
       </c>
       <c r="K41" s="0" t="n">
         <f aca="false">I41+J41</f>
-        <v>80.9</v>
+        <v>100.6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26107,10 +26104,10 @@
       </c>
       <c r="C42" s="0" t="n">
         <f aca="false">D41</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>1646</v>
@@ -26120,7 +26117,7 @@
       </c>
       <c r="G42" s="0" t="n">
         <f aca="false">MATCH(D42,'Rate calcs'!$A$24:$A$30,0)+IF(B42="Express",12,0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H42" s="0" t="n">
         <f aca="false">MATCH(A42,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26128,15 +26125,15 @@
       </c>
       <c r="I42" s="4" t="n">
         <f aca="false">IF(E42="Yes",(D42*'Rate calcs'!$C$8-100)/100*IF(A42="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="J42" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G42,H42)</f>
-        <v>72.6</v>
+        <v>81.3</v>
       </c>
       <c r="K42" s="0" t="n">
         <f aca="false">I42+J42</f>
-        <v>100.6</v>
+        <v>125.3</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26149,10 +26146,10 @@
       </c>
       <c r="C43" s="0" t="n">
         <f aca="false">D42</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E43" s="0" t="s">
         <v>1646</v>
@@ -26162,7 +26159,7 @@
       </c>
       <c r="G43" s="0" t="n">
         <f aca="false">MATCH(D43,'Rate calcs'!$A$24:$A$30,0)+IF(B43="Express",12,0)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H43" s="0" t="n">
         <f aca="false">MATCH(A43,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26170,31 +26167,29 @@
       </c>
       <c r="I43" s="4" t="n">
         <f aca="false">IF(E43="Yes",(D43*'Rate calcs'!$C$8-100)/100*IF(A43="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="J43" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G43,H43)</f>
-        <v>81.3</v>
+        <v>98.7</v>
       </c>
       <c r="K43" s="0" t="n">
         <f aca="false">I43+J43</f>
-        <v>125.3</v>
+        <v>174.7</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="str">
-        <f aca="false">A43</f>
-        <v>Zone 5</v>
+      <c r="A44" s="0" t="s">
+        <v>1613</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C44" s="0" t="n">
-        <f aca="false">D43</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="E44" s="0" t="s">
         <v>1646</v>
@@ -26204,37 +26199,39 @@
       </c>
       <c r="G44" s="0" t="n">
         <f aca="false">MATCH(D44,'Rate calcs'!$A$24:$A$30,0)+IF(B44="Express",12,0)</f>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H44" s="0" t="n">
         <f aca="false">MATCH(A44,'Rate calcs'!$B$23:$K$23,0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I44" s="4" t="n">
         <f aca="false">IF(E44="Yes",(D44*'Rate calcs'!$C$8-100)/100*IF(A44="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="J44" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G44,H44)</f>
-        <v>98.7</v>
+        <v>40.2</v>
       </c>
       <c r="K44" s="0" t="n">
         <f aca="false">I44+J44</f>
-        <v>174.7</v>
+        <v>40.2</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>1613</v>
+      <c r="A45" s="0" t="str">
+        <f aca="false">A44</f>
+        <v>Zone 6</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>0</v>
+        <f aca="false">D44</f>
+        <v>0.25</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E45" s="0" t="s">
         <v>1646</v>
@@ -26244,7 +26241,7 @@
       </c>
       <c r="G45" s="0" t="n">
         <f aca="false">MATCH(D45,'Rate calcs'!$A$24:$A$30,0)+IF(B45="Express",12,0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H45" s="0" t="n">
         <f aca="false">MATCH(A45,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26252,15 +26249,15 @@
       </c>
       <c r="I45" s="4" t="n">
         <f aca="false">IF(E45="Yes",(D45*'Rate calcs'!$C$8-100)/100*IF(A45="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J45" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G45,H45)</f>
-        <v>40.2</v>
+        <v>43.2</v>
       </c>
       <c r="K45" s="0" t="n">
         <f aca="false">I45+J45</f>
-        <v>40.2</v>
+        <v>47.2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26273,10 +26270,10 @@
       </c>
       <c r="C46" s="0" t="n">
         <f aca="false">D45</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E46" s="0" t="s">
         <v>1646</v>
@@ -26286,7 +26283,7 @@
       </c>
       <c r="G46" s="0" t="n">
         <f aca="false">MATCH(D46,'Rate calcs'!$A$24:$A$30,0)+IF(B46="Express",12,0)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H46" s="0" t="n">
         <f aca="false">MATCH(A46,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26294,15 +26291,15 @@
       </c>
       <c r="I46" s="4" t="n">
         <f aca="false">IF(E46="Yes",(D46*'Rate calcs'!$C$8-100)/100*IF(A46="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J46" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G46,H46)</f>
-        <v>43.2</v>
+        <v>56.1</v>
       </c>
       <c r="K46" s="0" t="n">
         <f aca="false">I46+J46</f>
-        <v>47.2</v>
+        <v>68.1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26315,10 +26312,10 @@
       </c>
       <c r="C47" s="0" t="n">
         <f aca="false">D46</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E47" s="0" t="s">
         <v>1646</v>
@@ -26328,7 +26325,7 @@
       </c>
       <c r="G47" s="0" t="n">
         <f aca="false">MATCH(D47,'Rate calcs'!$A$24:$A$30,0)+IF(B47="Express",12,0)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H47" s="0" t="n">
         <f aca="false">MATCH(A47,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26336,15 +26333,15 @@
       </c>
       <c r="I47" s="4" t="n">
         <f aca="false">IF(E47="Yes",(D47*'Rate calcs'!$C$8-100)/100*IF(A47="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J47" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G47,H47)</f>
-        <v>56.1</v>
+        <v>69</v>
       </c>
       <c r="K47" s="0" t="n">
         <f aca="false">I47+J47</f>
-        <v>68.1</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26357,10 +26354,10 @@
       </c>
       <c r="C48" s="0" t="n">
         <f aca="false">D47</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E48" s="0" t="s">
         <v>1646</v>
@@ -26370,7 +26367,7 @@
       </c>
       <c r="G48" s="0" t="n">
         <f aca="false">MATCH(D48,'Rate calcs'!$A$24:$A$30,0)+IF(B48="Express",12,0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H48" s="0" t="n">
         <f aca="false">MATCH(A48,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26378,15 +26375,15 @@
       </c>
       <c r="I48" s="4" t="n">
         <f aca="false">IF(E48="Yes",(D48*'Rate calcs'!$C$8-100)/100*IF(A48="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J48" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G48,H48)</f>
-        <v>69</v>
+        <v>81.9</v>
       </c>
       <c r="K48" s="0" t="n">
         <f aca="false">I48+J48</f>
-        <v>89</v>
+        <v>109.9</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26399,10 +26396,10 @@
       </c>
       <c r="C49" s="0" t="n">
         <f aca="false">D48</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E49" s="0" t="s">
         <v>1646</v>
@@ -26412,7 +26409,7 @@
       </c>
       <c r="G49" s="0" t="n">
         <f aca="false">MATCH(D49,'Rate calcs'!$A$24:$A$30,0)+IF(B49="Express",12,0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H49" s="0" t="n">
         <f aca="false">MATCH(A49,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26420,15 +26417,15 @@
       </c>
       <c r="I49" s="4" t="n">
         <f aca="false">IF(E49="Yes",(D49*'Rate calcs'!$C$8-100)/100*IF(A49="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="J49" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G49,H49)</f>
-        <v>81.9</v>
+        <v>90.7</v>
       </c>
       <c r="K49" s="0" t="n">
         <f aca="false">I49+J49</f>
-        <v>109.9</v>
+        <v>134.7</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26441,10 +26438,10 @@
       </c>
       <c r="C50" s="0" t="n">
         <f aca="false">D49</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E50" s="0" t="s">
         <v>1646</v>
@@ -26454,7 +26451,7 @@
       </c>
       <c r="G50" s="0" t="n">
         <f aca="false">MATCH(D50,'Rate calcs'!$A$24:$A$30,0)+IF(B50="Express",12,0)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H50" s="0" t="n">
         <f aca="false">MATCH(A50,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26462,31 +26459,29 @@
       </c>
       <c r="I50" s="4" t="n">
         <f aca="false">IF(E50="Yes",(D50*'Rate calcs'!$C$8-100)/100*IF(A50="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="J50" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G50,H50)</f>
-        <v>90.7</v>
+        <v>108.3</v>
       </c>
       <c r="K50" s="0" t="n">
         <f aca="false">I50+J50</f>
-        <v>134.7</v>
+        <v>184.3</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="str">
-        <f aca="false">A50</f>
-        <v>Zone 6</v>
+      <c r="A51" s="0" t="s">
+        <v>1614</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C51" s="0" t="n">
-        <f aca="false">D50</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>1646</v>
@@ -26496,37 +26491,39 @@
       </c>
       <c r="G51" s="0" t="n">
         <f aca="false">MATCH(D51,'Rate calcs'!$A$24:$A$30,0)+IF(B51="Express",12,0)</f>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H51" s="0" t="n">
         <f aca="false">MATCH(A51,'Rate calcs'!$B$23:$K$23,0)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I51" s="4" t="n">
         <f aca="false">IF(E51="Yes",(D51*'Rate calcs'!$C$8-100)/100*IF(A51="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="J51" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G51,H51)</f>
-        <v>108.3</v>
+        <v>41.3</v>
       </c>
       <c r="K51" s="0" t="n">
         <f aca="false">I51+J51</f>
-        <v>184.3</v>
+        <v>41.3</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>1614</v>
+      <c r="A52" s="0" t="str">
+        <f aca="false">A51</f>
+        <v>Zone 7</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>0</v>
+        <f aca="false">D51</f>
+        <v>0.25</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>1646</v>
@@ -26536,7 +26533,7 @@
       </c>
       <c r="G52" s="0" t="n">
         <f aca="false">MATCH(D52,'Rate calcs'!$A$24:$A$30,0)+IF(B52="Express",12,0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H52" s="0" t="n">
         <f aca="false">MATCH(A52,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26544,15 +26541,15 @@
       </c>
       <c r="I52" s="4" t="n">
         <f aca="false">IF(E52="Yes",(D52*'Rate calcs'!$C$8-100)/100*IF(A52="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J52" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G52,H52)</f>
-        <v>41.3</v>
+        <v>44.3</v>
       </c>
       <c r="K52" s="0" t="n">
         <f aca="false">I52+J52</f>
-        <v>41.3</v>
+        <v>48.3</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26565,10 +26562,10 @@
       </c>
       <c r="C53" s="0" t="n">
         <f aca="false">D52</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E53" s="0" t="s">
         <v>1646</v>
@@ -26578,7 +26575,7 @@
       </c>
       <c r="G53" s="0" t="n">
         <f aca="false">MATCH(D53,'Rate calcs'!$A$24:$A$30,0)+IF(B53="Express",12,0)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H53" s="0" t="n">
         <f aca="false">MATCH(A53,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26586,15 +26583,15 @@
       </c>
       <c r="I53" s="4" t="n">
         <f aca="false">IF(E53="Yes",(D53*'Rate calcs'!$C$8-100)/100*IF(A53="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J53" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G53,H53)</f>
-        <v>44.3</v>
+        <v>57.2</v>
       </c>
       <c r="K53" s="0" t="n">
         <f aca="false">I53+J53</f>
-        <v>48.3</v>
+        <v>69.2</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26607,10 +26604,10 @@
       </c>
       <c r="C54" s="0" t="n">
         <f aca="false">D53</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E54" s="0" t="s">
         <v>1646</v>
@@ -26620,7 +26617,7 @@
       </c>
       <c r="G54" s="0" t="n">
         <f aca="false">MATCH(D54,'Rate calcs'!$A$24:$A$30,0)+IF(B54="Express",12,0)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H54" s="0" t="n">
         <f aca="false">MATCH(A54,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26628,15 +26625,15 @@
       </c>
       <c r="I54" s="4" t="n">
         <f aca="false">IF(E54="Yes",(D54*'Rate calcs'!$C$8-100)/100*IF(A54="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J54" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G54,H54)</f>
-        <v>57.2</v>
+        <v>70.1</v>
       </c>
       <c r="K54" s="0" t="n">
         <f aca="false">I54+J54</f>
-        <v>69.2</v>
+        <v>90.1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26649,10 +26646,10 @@
       </c>
       <c r="C55" s="0" t="n">
         <f aca="false">D54</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E55" s="0" t="s">
         <v>1646</v>
@@ -26662,7 +26659,7 @@
       </c>
       <c r="G55" s="0" t="n">
         <f aca="false">MATCH(D55,'Rate calcs'!$A$24:$A$30,0)+IF(B55="Express",12,0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H55" s="0" t="n">
         <f aca="false">MATCH(A55,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26670,15 +26667,15 @@
       </c>
       <c r="I55" s="4" t="n">
         <f aca="false">IF(E55="Yes",(D55*'Rate calcs'!$C$8-100)/100*IF(A55="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J55" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G55,H55)</f>
-        <v>70.1</v>
+        <v>83</v>
       </c>
       <c r="K55" s="0" t="n">
         <f aca="false">I55+J55</f>
-        <v>90.1</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26691,10 +26688,10 @@
       </c>
       <c r="C56" s="0" t="n">
         <f aca="false">D55</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>1646</v>
@@ -26704,7 +26701,7 @@
       </c>
       <c r="G56" s="0" t="n">
         <f aca="false">MATCH(D56,'Rate calcs'!$A$24:$A$30,0)+IF(B56="Express",12,0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H56" s="0" t="n">
         <f aca="false">MATCH(A56,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26712,15 +26709,15 @@
       </c>
       <c r="I56" s="4" t="n">
         <f aca="false">IF(E56="Yes",(D56*'Rate calcs'!$C$8-100)/100*IF(A56="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="J56" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G56,H56)</f>
-        <v>83</v>
+        <v>91.8</v>
       </c>
       <c r="K56" s="0" t="n">
         <f aca="false">I56+J56</f>
-        <v>111</v>
+        <v>135.8</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26733,10 +26730,10 @@
       </c>
       <c r="C57" s="0" t="n">
         <f aca="false">D56</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E57" s="0" t="s">
         <v>1646</v>
@@ -26746,7 +26743,7 @@
       </c>
       <c r="G57" s="0" t="n">
         <f aca="false">MATCH(D57,'Rate calcs'!$A$24:$A$30,0)+IF(B57="Express",12,0)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H57" s="0" t="n">
         <f aca="false">MATCH(A57,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26754,31 +26751,29 @@
       </c>
       <c r="I57" s="4" t="n">
         <f aca="false">IF(E57="Yes",(D57*'Rate calcs'!$C$8-100)/100*IF(A57="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="J57" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G57,H57)</f>
-        <v>91.8</v>
+        <v>109.4</v>
       </c>
       <c r="K57" s="0" t="n">
         <f aca="false">I57+J57</f>
-        <v>135.8</v>
+        <v>185.4</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="str">
-        <f aca="false">A57</f>
-        <v>Zone 7</v>
+      <c r="A58" s="0" t="s">
+        <v>1615</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C58" s="0" t="n">
-        <f aca="false">D57</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="E58" s="0" t="s">
         <v>1646</v>
@@ -26788,37 +26783,39 @@
       </c>
       <c r="G58" s="0" t="n">
         <f aca="false">MATCH(D58,'Rate calcs'!$A$24:$A$30,0)+IF(B58="Express",12,0)</f>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H58" s="0" t="n">
         <f aca="false">MATCH(A58,'Rate calcs'!$B$23:$K$23,0)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I58" s="4" t="n">
         <f aca="false">IF(E58="Yes",(D58*'Rate calcs'!$C$8-100)/100*IF(A58="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="J58" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G58,H58)</f>
-        <v>109.4</v>
+        <v>43.8</v>
       </c>
       <c r="K58" s="0" t="n">
         <f aca="false">I58+J58</f>
-        <v>185.4</v>
+        <v>43.8</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>1615</v>
+      <c r="A59" s="0" t="str">
+        <f aca="false">A58</f>
+        <v>Zone 8</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>0</v>
+        <f aca="false">D58</f>
+        <v>0.25</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E59" s="0" t="s">
         <v>1646</v>
@@ -26828,7 +26825,7 @@
       </c>
       <c r="G59" s="0" t="n">
         <f aca="false">MATCH(D59,'Rate calcs'!$A$24:$A$30,0)+IF(B59="Express",12,0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H59" s="0" t="n">
         <f aca="false">MATCH(A59,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26836,15 +26833,15 @@
       </c>
       <c r="I59" s="4" t="n">
         <f aca="false">IF(E59="Yes",(D59*'Rate calcs'!$C$8-100)/100*IF(A59="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J59" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G59,H59)</f>
-        <v>43.8</v>
+        <v>46.8</v>
       </c>
       <c r="K59" s="0" t="n">
         <f aca="false">I59+J59</f>
-        <v>43.8</v>
+        <v>50.8</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26857,10 +26854,10 @@
       </c>
       <c r="C60" s="0" t="n">
         <f aca="false">D59</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>1646</v>
@@ -26870,7 +26867,7 @@
       </c>
       <c r="G60" s="0" t="n">
         <f aca="false">MATCH(D60,'Rate calcs'!$A$24:$A$30,0)+IF(B60="Express",12,0)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H60" s="0" t="n">
         <f aca="false">MATCH(A60,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26878,15 +26875,15 @@
       </c>
       <c r="I60" s="4" t="n">
         <f aca="false">IF(E60="Yes",(D60*'Rate calcs'!$C$8-100)/100*IF(A60="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J60" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G60,H60)</f>
-        <v>46.8</v>
+        <v>63.35</v>
       </c>
       <c r="K60" s="0" t="n">
         <f aca="false">I60+J60</f>
-        <v>50.8</v>
+        <v>75.35</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26899,10 +26896,10 @@
       </c>
       <c r="C61" s="0" t="n">
         <f aca="false">D60</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>1646</v>
@@ -26912,7 +26909,7 @@
       </c>
       <c r="G61" s="0" t="n">
         <f aca="false">MATCH(D61,'Rate calcs'!$A$24:$A$30,0)+IF(B61="Express",12,0)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H61" s="0" t="n">
         <f aca="false">MATCH(A61,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26920,15 +26917,15 @@
       </c>
       <c r="I61" s="4" t="n">
         <f aca="false">IF(E61="Yes",(D61*'Rate calcs'!$C$8-100)/100*IF(A61="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J61" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G61,H61)</f>
-        <v>63.35</v>
+        <v>79.9</v>
       </c>
       <c r="K61" s="0" t="n">
         <f aca="false">I61+J61</f>
-        <v>75.35</v>
+        <v>99.9</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26941,10 +26938,10 @@
       </c>
       <c r="C62" s="0" t="n">
         <f aca="false">D61</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>1646</v>
@@ -26954,7 +26951,7 @@
       </c>
       <c r="G62" s="0" t="n">
         <f aca="false">MATCH(D62,'Rate calcs'!$A$24:$A$30,0)+IF(B62="Express",12,0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H62" s="0" t="n">
         <f aca="false">MATCH(A62,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -26962,15 +26959,15 @@
       </c>
       <c r="I62" s="4" t="n">
         <f aca="false">IF(E62="Yes",(D62*'Rate calcs'!$C$8-100)/100*IF(A62="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J62" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G62,H62)</f>
-        <v>79.9</v>
+        <v>96.45</v>
       </c>
       <c r="K62" s="0" t="n">
         <f aca="false">I62+J62</f>
-        <v>99.9</v>
+        <v>124.45</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26983,10 +26980,10 @@
       </c>
       <c r="C63" s="0" t="n">
         <f aca="false">D62</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E63" s="0" t="s">
         <v>1646</v>
@@ -26996,7 +26993,7 @@
       </c>
       <c r="G63" s="0" t="n">
         <f aca="false">MATCH(D63,'Rate calcs'!$A$24:$A$30,0)+IF(B63="Express",12,0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H63" s="0" t="n">
         <f aca="false">MATCH(A63,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -27004,15 +27001,15 @@
       </c>
       <c r="I63" s="4" t="n">
         <f aca="false">IF(E63="Yes",(D63*'Rate calcs'!$C$8-100)/100*IF(A63="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="J63" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G63,H63)</f>
-        <v>96.45</v>
+        <v>113.15</v>
       </c>
       <c r="K63" s="0" t="n">
         <f aca="false">I63+J63</f>
-        <v>124.45</v>
+        <v>157.15</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27025,10 +27022,10 @@
       </c>
       <c r="C64" s="0" t="n">
         <f aca="false">D63</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E64" s="0" t="s">
         <v>1646</v>
@@ -27038,7 +27035,7 @@
       </c>
       <c r="G64" s="0" t="n">
         <f aca="false">MATCH(D64,'Rate calcs'!$A$24:$A$30,0)+IF(B64="Express",12,0)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H64" s="0" t="n">
         <f aca="false">MATCH(A64,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -27046,31 +27043,29 @@
       </c>
       <c r="I64" s="4" t="n">
         <f aca="false">IF(E64="Yes",(D64*'Rate calcs'!$C$8-100)/100*IF(A64="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="J64" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G64,H64)</f>
-        <v>113.15</v>
+        <v>146.55</v>
       </c>
       <c r="K64" s="0" t="n">
         <f aca="false">I64+J64</f>
-        <v>157.15</v>
+        <v>222.55</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="str">
-        <f aca="false">A64</f>
-        <v>Zone 8</v>
+      <c r="A65" s="0" t="s">
+        <v>1616</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C65" s="0" t="n">
-        <f aca="false">D64</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="E65" s="0" t="s">
         <v>1646</v>
@@ -27080,37 +27075,39 @@
       </c>
       <c r="G65" s="0" t="n">
         <f aca="false">MATCH(D65,'Rate calcs'!$A$24:$A$30,0)+IF(B65="Express",12,0)</f>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H65" s="0" t="n">
         <f aca="false">MATCH(A65,'Rate calcs'!$B$23:$K$23,0)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I65" s="4" t="n">
         <f aca="false">IF(E65="Yes",(D65*'Rate calcs'!$C$8-100)/100*IF(A65="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="J65" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G65,H65)</f>
-        <v>146.55</v>
+        <v>45.15</v>
       </c>
       <c r="K65" s="0" t="n">
         <f aca="false">I65+J65</f>
-        <v>222.55</v>
+        <v>45.15</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>1616</v>
+      <c r="A66" s="0" t="str">
+        <f aca="false">A65</f>
+        <v>Zone 9</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>1617</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>0</v>
+        <f aca="false">D65</f>
+        <v>0.25</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E66" s="0" t="s">
         <v>1646</v>
@@ -27120,7 +27117,7 @@
       </c>
       <c r="G66" s="0" t="n">
         <f aca="false">MATCH(D66,'Rate calcs'!$A$24:$A$30,0)+IF(B66="Express",12,0)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H66" s="0" t="n">
         <f aca="false">MATCH(A66,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -27128,15 +27125,15 @@
       </c>
       <c r="I66" s="4" t="n">
         <f aca="false">IF(E66="Yes",(D66*'Rate calcs'!$C$8-100)/100*IF(A66="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J66" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G66,H66)</f>
-        <v>45.15</v>
+        <v>48.15</v>
       </c>
       <c r="K66" s="0" t="n">
         <f aca="false">I66+J66</f>
-        <v>45.15</v>
+        <v>52.15</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27149,10 +27146,10 @@
       </c>
       <c r="C67" s="0" t="n">
         <f aca="false">D66</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E67" s="0" t="s">
         <v>1646</v>
@@ -27162,7 +27159,7 @@
       </c>
       <c r="G67" s="0" t="n">
         <f aca="false">MATCH(D67,'Rate calcs'!$A$24:$A$30,0)+IF(B67="Express",12,0)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H67" s="0" t="n">
         <f aca="false">MATCH(A67,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -27170,15 +27167,15 @@
       </c>
       <c r="I67" s="4" t="n">
         <f aca="false">IF(E67="Yes",(D67*'Rate calcs'!$C$8-100)/100*IF(A67="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J67" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G67,H67)</f>
-        <v>48.15</v>
+        <v>64.7</v>
       </c>
       <c r="K67" s="0" t="n">
         <f aca="false">I67+J67</f>
-        <v>52.15</v>
+        <v>76.7</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27191,10 +27188,10 @@
       </c>
       <c r="C68" s="0" t="n">
         <f aca="false">D67</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>1646</v>
@@ -27204,7 +27201,7 @@
       </c>
       <c r="G68" s="0" t="n">
         <f aca="false">MATCH(D68,'Rate calcs'!$A$24:$A$30,0)+IF(B68="Express",12,0)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H68" s="0" t="n">
         <f aca="false">MATCH(A68,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -27212,15 +27209,15 @@
       </c>
       <c r="I68" s="4" t="n">
         <f aca="false">IF(E68="Yes",(D68*'Rate calcs'!$C$8-100)/100*IF(A68="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J68" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G68,H68)</f>
-        <v>64.7</v>
+        <v>81.25</v>
       </c>
       <c r="K68" s="0" t="n">
         <f aca="false">I68+J68</f>
-        <v>76.7</v>
+        <v>101.25</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27233,10 +27230,10 @@
       </c>
       <c r="C69" s="0" t="n">
         <f aca="false">D68</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E69" s="0" t="s">
         <v>1646</v>
@@ -27246,7 +27243,7 @@
       </c>
       <c r="G69" s="0" t="n">
         <f aca="false">MATCH(D69,'Rate calcs'!$A$24:$A$30,0)+IF(B69="Express",12,0)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H69" s="0" t="n">
         <f aca="false">MATCH(A69,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -27254,15 +27251,15 @@
       </c>
       <c r="I69" s="4" t="n">
         <f aca="false">IF(E69="Yes",(D69*'Rate calcs'!$C$8-100)/100*IF(A69="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J69" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G69,H69)</f>
-        <v>81.25</v>
+        <v>97.8</v>
       </c>
       <c r="K69" s="0" t="n">
         <f aca="false">I69+J69</f>
-        <v>101.25</v>
+        <v>125.8</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27275,10 +27272,10 @@
       </c>
       <c r="C70" s="0" t="n">
         <f aca="false">D69</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E70" s="0" t="s">
         <v>1646</v>
@@ -27288,7 +27285,7 @@
       </c>
       <c r="G70" s="0" t="n">
         <f aca="false">MATCH(D70,'Rate calcs'!$A$24:$A$30,0)+IF(B70="Express",12,0)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H70" s="0" t="n">
         <f aca="false">MATCH(A70,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -27296,15 +27293,15 @@
       </c>
       <c r="I70" s="4" t="n">
         <f aca="false">IF(E70="Yes",(D70*'Rate calcs'!$C$8-100)/100*IF(A70="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="J70" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G70,H70)</f>
-        <v>97.8</v>
+        <v>114.5</v>
       </c>
       <c r="K70" s="0" t="n">
         <f aca="false">I70+J70</f>
-        <v>125.8</v>
+        <v>158.5</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27317,10 +27314,10 @@
       </c>
       <c r="C71" s="0" t="n">
         <f aca="false">D70</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E71" s="0" t="s">
         <v>1646</v>
@@ -27330,7 +27327,7 @@
       </c>
       <c r="G71" s="0" t="n">
         <f aca="false">MATCH(D71,'Rate calcs'!$A$24:$A$30,0)+IF(B71="Express",12,0)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H71" s="0" t="n">
         <f aca="false">MATCH(A71,'Rate calcs'!$B$23:$K$23,0)</f>
@@ -27338,63 +27335,21 @@
       </c>
       <c r="I71" s="4" t="n">
         <f aca="false">IF(E71="Yes",(D71*'Rate calcs'!$C$8-100)/100*IF(A71="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="J71" s="4" t="n">
         <f aca="true">OFFSET('Rate calcs'!$A$23,G71,H71)</f>
-        <v>114.5</v>
+        <v>147.9</v>
       </c>
       <c r="K71" s="0" t="n">
         <f aca="false">I71+J71</f>
-        <v>158.5</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="str">
-        <f aca="false">A71</f>
-        <v>Zone 9</v>
-      </c>
-      <c r="B72" s="0" t="s">
-        <v>1617</v>
-      </c>
-      <c r="C72" s="0" t="n">
-        <f aca="false">D71</f>
-        <v>3</v>
-      </c>
-      <c r="D72" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>1646</v>
-      </c>
-      <c r="F72" s="0" t="s">
-        <v>1648</v>
-      </c>
-      <c r="G72" s="0" t="n">
-        <f aca="false">MATCH(D72,'Rate calcs'!$A$24:$A$30,0)+IF(B72="Express",12,0)</f>
-        <v>19</v>
-      </c>
-      <c r="H72" s="0" t="n">
-        <f aca="false">MATCH(A72,'Rate calcs'!$B$23:$K$23,0)</f>
-        <v>10</v>
-      </c>
-      <c r="I72" s="4" t="n">
-        <f aca="false">IF(E72="Yes",(D72*'Rate calcs'!$C$8-100)/100*IF(A72="Domestic",'Rate calcs'!$C$17,'Rate calcs'!$C$18),0)</f>
-        <v>76</v>
-      </c>
-      <c r="J72" s="4" t="n">
-        <f aca="true">OFFSET('Rate calcs'!$A$23,G72,H72)</f>
-        <v>147.9</v>
-      </c>
-      <c r="K72" s="0" t="n">
-        <f aca="false">I72+J72</f>
         <v>223.9</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -27407,16 +27362,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="11.52"/>
@@ -27904,23 +27859,23 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A23,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 2: China</v>
+        <v>Zone 3: Rest of Asia</v>
       </c>
       <c r="B23" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F23</f>
-        <v>International Express (1kg)</v>
+        <v>International Insured Express</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C23=0,0,'Rate definitions 2'!C23+0.001)</f>
-        <v>5.001</v>
+        <v>0</v>
       </c>
       <c r="D23" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D23+0.001</f>
-        <v>1.001</v>
+        <v>0.251</v>
       </c>
       <c r="E23" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K23</f>
-        <v>47.9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27934,15 +27889,15 @@
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C24=0,0,'Rate definitions 2'!C24+0.001)</f>
-        <v>0</v>
+        <v>0.251</v>
       </c>
       <c r="D24" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D24+0.001</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="E24" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K24</f>
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27956,15 +27911,15 @@
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C25=0,0,'Rate definitions 2'!C25+0.001)</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="D25" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D25+0.001</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="E25" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K25</f>
-        <v>41</v>
+        <v>60.7</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27978,15 +27933,15 @@
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C26=0,0,'Rate definitions 2'!C26+0.001)</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="D26" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D26+0.001</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="E26" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K26</f>
-        <v>60.7</v>
+        <v>80.4</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28000,15 +27955,15 @@
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C27=0,0,'Rate definitions 2'!C27+0.001)</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="D27" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D27+0.001</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="E27" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K27</f>
-        <v>80.4</v>
+        <v>100.1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28022,15 +27977,15 @@
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C28=0,0,'Rate definitions 2'!C28+0.001)</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="D28" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D28+0.001</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="E28" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K28</f>
-        <v>100.1</v>
+        <v>124.8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28044,21 +27999,21 @@
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C29=0,0,'Rate definitions 2'!C29+0.001)</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="D29" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D29+0.001</f>
-        <v>3.001</v>
+        <v>5.001</v>
       </c>
       <c r="E29" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K29</f>
-        <v>124.8</v>
+        <v>174.2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A30,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 3: Rest of Asia</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B30" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F30</f>
@@ -28066,21 +28021,21 @@
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C30=0,0,'Rate definitions 2'!C30+0.001)</f>
-        <v>3.001</v>
+        <v>0</v>
       </c>
       <c r="D30" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D30+0.001</f>
-        <v>5.001</v>
+        <v>0.251</v>
       </c>
       <c r="E30" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K30</f>
-        <v>174.2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A31,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B31" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F31</f>
@@ -28088,21 +28043,21 @@
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C31=0,0,'Rate definitions 2'!C31+0.001)</f>
-        <v>0</v>
+        <v>0.251</v>
       </c>
       <c r="D31" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D31+0.001</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="E31" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K31</f>
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A32,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B32" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F32</f>
@@ -28110,21 +28065,21 @@
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C32=0,0,'Rate definitions 2'!C32+0.001)</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="D32" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D32+0.001</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="E32" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K32</f>
-        <v>43</v>
+        <v>63.9</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A33,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B33" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F33</f>
@@ -28132,21 +28087,21 @@
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C33=0,0,'Rate definitions 2'!C33+0.001)</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="D33" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D33+0.001</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="E33" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K33</f>
-        <v>63.9</v>
+        <v>84.8</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A34,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B34" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F34</f>
@@ -28154,21 +28109,21 @@
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C34=0,0,'Rate definitions 2'!C34+0.001)</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="D34" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D34+0.001</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="E34" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K34</f>
-        <v>84.8</v>
+        <v>105.7</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A35,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B35" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F35</f>
@@ -28176,21 +28131,21 @@
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C35=0,0,'Rate definitions 2'!C35+0.001)</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="D35" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D35+0.001</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="E35" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K35</f>
-        <v>105.7</v>
+        <v>130.5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A36,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 4: USA &amp; Canada</v>
       </c>
       <c r="B36" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F36</f>
@@ -28198,21 +28153,21 @@
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C36=0,0,'Rate definitions 2'!C36+0.001)</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="D36" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D36+0.001</f>
-        <v>3.001</v>
+        <v>5.001</v>
       </c>
       <c r="E36" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K36</f>
-        <v>130.5</v>
+        <v>180.1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A37,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 4: USA and Canada</v>
+        <v>Zone 5: Pacific islands</v>
       </c>
       <c r="B37" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F37</f>
@@ -28220,15 +28175,15 @@
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C37=0,0,'Rate definitions 2'!C37+0.001)</f>
-        <v>3.001</v>
+        <v>0</v>
       </c>
       <c r="D37" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D37+0.001</f>
-        <v>5.001</v>
+        <v>0.251</v>
       </c>
       <c r="E37" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K37</f>
-        <v>180.1</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28242,15 +28197,15 @@
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C38=0,0,'Rate definitions 2'!C38+0.001)</f>
-        <v>0</v>
+        <v>0.251</v>
       </c>
       <c r="D38" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D38+0.001</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="E38" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K38</f>
-        <v>34.5</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28264,15 +28219,15 @@
       </c>
       <c r="C39" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C39=0,0,'Rate definitions 2'!C39+0.001)</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="D39" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D39+0.001</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="E39" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K39</f>
-        <v>41.5</v>
+        <v>61.2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28286,15 +28241,15 @@
       </c>
       <c r="C40" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C40=0,0,'Rate definitions 2'!C40+0.001)</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="D40" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D40+0.001</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="E40" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K40</f>
-        <v>61.2</v>
+        <v>80.9</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28308,15 +28263,15 @@
       </c>
       <c r="C41" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C41=0,0,'Rate definitions 2'!C41+0.001)</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="D41" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D41+0.001</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="E41" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K41</f>
-        <v>80.9</v>
+        <v>100.6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28330,15 +28285,15 @@
       </c>
       <c r="C42" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C42=0,0,'Rate definitions 2'!C42+0.001)</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="D42" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D42+0.001</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="E42" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K42</f>
-        <v>100.6</v>
+        <v>125.3</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28352,21 +28307,21 @@
       </c>
       <c r="C43" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C43=0,0,'Rate definitions 2'!C43+0.001)</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="D43" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D43+0.001</f>
-        <v>3.001</v>
+        <v>5.001</v>
       </c>
       <c r="E43" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K43</f>
-        <v>125.3</v>
+        <v>174.7</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A44,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 5: Pacific islands</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B44" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F44</f>
@@ -28374,21 +28329,21 @@
       </c>
       <c r="C44" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C44=0,0,'Rate definitions 2'!C44+0.001)</f>
-        <v>3.001</v>
+        <v>0</v>
       </c>
       <c r="D44" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D44+0.001</f>
-        <v>5.001</v>
+        <v>0.251</v>
       </c>
       <c r="E44" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K44</f>
-        <v>174.7</v>
+        <v>40.2</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A45,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B45" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F45</f>
@@ -28396,21 +28351,21 @@
       </c>
       <c r="C45" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C45=0,0,'Rate definitions 2'!C45+0.001)</f>
-        <v>0</v>
+        <v>0.251</v>
       </c>
       <c r="D45" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D45+0.001</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="E45" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K45</f>
-        <v>40.2</v>
+        <v>47.2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A46,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B46" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F46</f>
@@ -28418,21 +28373,21 @@
       </c>
       <c r="C46" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C46=0,0,'Rate definitions 2'!C46+0.001)</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="D46" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D46+0.001</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="E46" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K46</f>
-        <v>47.2</v>
+        <v>68.1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A47,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B47" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F47</f>
@@ -28440,21 +28395,21 @@
       </c>
       <c r="C47" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C47=0,0,'Rate definitions 2'!C47+0.001)</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="D47" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D47+0.001</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="E47" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K47</f>
-        <v>68.1</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A48,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B48" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F48</f>
@@ -28462,21 +28417,21 @@
       </c>
       <c r="C48" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C48=0,0,'Rate definitions 2'!C48+0.001)</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="D48" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D48+0.001</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="E48" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K48</f>
-        <v>89</v>
+        <v>109.9</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A49,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B49" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F49</f>
@@ -28484,21 +28439,21 @@
       </c>
       <c r="C49" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C49=0,0,'Rate definitions 2'!C49+0.001)</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="D49" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D49+0.001</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="E49" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K49</f>
-        <v>109.9</v>
+        <v>134.7</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A50,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 6: UK &amp; Ireland</v>
       </c>
       <c r="B50" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F50</f>
@@ -28506,21 +28461,21 @@
       </c>
       <c r="C50" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C50=0,0,'Rate definitions 2'!C50+0.001)</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="D50" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D50+0.001</f>
-        <v>3.001</v>
+        <v>5.001</v>
       </c>
       <c r="E50" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K50</f>
-        <v>134.7</v>
+        <v>184.3</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A51,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 6: UK and Ireland</v>
+        <v>Zone 7: Major Europe</v>
       </c>
       <c r="B51" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F51</f>
@@ -28528,15 +28483,15 @@
       </c>
       <c r="C51" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C51=0,0,'Rate definitions 2'!C51+0.001)</f>
-        <v>3.001</v>
+        <v>0</v>
       </c>
       <c r="D51" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D51+0.001</f>
-        <v>5.001</v>
+        <v>0.251</v>
       </c>
       <c r="E51" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K51</f>
-        <v>184.3</v>
+        <v>41.3</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28550,15 +28505,15 @@
       </c>
       <c r="C52" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C52=0,0,'Rate definitions 2'!C52+0.001)</f>
-        <v>0</v>
+        <v>0.251</v>
       </c>
       <c r="D52" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D52+0.001</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="E52" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K52</f>
-        <v>41.3</v>
+        <v>48.3</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28572,15 +28527,15 @@
       </c>
       <c r="C53" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C53=0,0,'Rate definitions 2'!C53+0.001)</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="D53" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D53+0.001</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="E53" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K53</f>
-        <v>48.3</v>
+        <v>69.2</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28594,15 +28549,15 @@
       </c>
       <c r="C54" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C54=0,0,'Rate definitions 2'!C54+0.001)</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="D54" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D54+0.001</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="E54" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K54</f>
-        <v>69.2</v>
+        <v>90.1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28616,15 +28571,15 @@
       </c>
       <c r="C55" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C55=0,0,'Rate definitions 2'!C55+0.001)</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="D55" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D55+0.001</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="E55" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K55</f>
-        <v>90.1</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28638,15 +28593,15 @@
       </c>
       <c r="C56" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C56=0,0,'Rate definitions 2'!C56+0.001)</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="D56" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D56+0.001</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="E56" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K56</f>
-        <v>111</v>
+        <v>135.8</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28660,21 +28615,21 @@
       </c>
       <c r="C57" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C57=0,0,'Rate definitions 2'!C57+0.001)</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="D57" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D57+0.001</f>
-        <v>3.001</v>
+        <v>5.001</v>
       </c>
       <c r="E57" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K57</f>
-        <v>135.8</v>
+        <v>185.4</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A58,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 7: Major Europe</v>
+        <v>Zone 8: Rest of World 1</v>
       </c>
       <c r="B58" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F58</f>
@@ -28682,15 +28637,15 @@
       </c>
       <c r="C58" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C58=0,0,'Rate definitions 2'!C58+0.001)</f>
-        <v>3.001</v>
+        <v>0</v>
       </c>
       <c r="D58" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D58+0.001</f>
-        <v>5.001</v>
+        <v>0.251</v>
       </c>
       <c r="E58" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K58</f>
-        <v>185.4</v>
+        <v>43.8</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28704,15 +28659,15 @@
       </c>
       <c r="C59" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C59=0,0,'Rate definitions 2'!C59+0.001)</f>
-        <v>0</v>
+        <v>0.251</v>
       </c>
       <c r="D59" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D59+0.001</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="E59" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K59</f>
-        <v>43.8</v>
+        <v>50.8</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28726,15 +28681,15 @@
       </c>
       <c r="C60" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C60=0,0,'Rate definitions 2'!C60+0.001)</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D60+0.001</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="E60" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K60</f>
-        <v>50.8</v>
+        <v>75.35</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28748,15 +28703,15 @@
       </c>
       <c r="C61" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C61=0,0,'Rate definitions 2'!C61+0.001)</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="D61" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D61+0.001</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="E61" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K61</f>
-        <v>75.35</v>
+        <v>99.9</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28770,15 +28725,15 @@
       </c>
       <c r="C62" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C62=0,0,'Rate definitions 2'!C62+0.001)</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="D62" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D62+0.001</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="E62" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K62</f>
-        <v>99.9</v>
+        <v>124.45</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28792,15 +28747,15 @@
       </c>
       <c r="C63" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C63=0,0,'Rate definitions 2'!C63+0.001)</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="D63" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D63+0.001</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="E63" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K63</f>
-        <v>124.45</v>
+        <v>157.15</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28814,21 +28769,21 @@
       </c>
       <c r="C64" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C64=0,0,'Rate definitions 2'!C64+0.001)</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="D64" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D64+0.001</f>
-        <v>3.001</v>
+        <v>5.001</v>
       </c>
       <c r="E64" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K64</f>
-        <v>157.15</v>
+        <v>222.55</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="str">
         <f aca="false">VLOOKUP('Rate definitions 2'!A65,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 8: Rest of World 1</v>
+        <v>Zone 9: Rest of World 2</v>
       </c>
       <c r="B65" s="0" t="str">
         <f aca="false">'Rate definitions 2'!F65</f>
@@ -28836,15 +28791,15 @@
       </c>
       <c r="C65" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C65=0,0,'Rate definitions 2'!C65+0.001)</f>
-        <v>3.001</v>
+        <v>0</v>
       </c>
       <c r="D65" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D65+0.001</f>
-        <v>5.001</v>
+        <v>0.251</v>
       </c>
       <c r="E65" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K65</f>
-        <v>222.55</v>
+        <v>45.15</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28858,15 +28813,15 @@
       </c>
       <c r="C66" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C66=0,0,'Rate definitions 2'!C66+0.001)</f>
-        <v>0</v>
+        <v>0.251</v>
       </c>
       <c r="D66" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D66+0.001</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="E66" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K66</f>
-        <v>45.15</v>
+        <v>52.15</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28880,15 +28835,15 @@
       </c>
       <c r="C67" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C67=0,0,'Rate definitions 2'!C67+0.001)</f>
-        <v>0.251</v>
+        <v>0.501</v>
       </c>
       <c r="D67" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D67+0.001</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="E67" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K67</f>
-        <v>52.15</v>
+        <v>76.7</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28902,15 +28857,15 @@
       </c>
       <c r="C68" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C68=0,0,'Rate definitions 2'!C68+0.001)</f>
-        <v>0.501</v>
+        <v>1.001</v>
       </c>
       <c r="D68" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D68+0.001</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="E68" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K68</f>
-        <v>76.7</v>
+        <v>101.25</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28924,15 +28879,15 @@
       </c>
       <c r="C69" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C69=0,0,'Rate definitions 2'!C69+0.001)</f>
-        <v>1.001</v>
+        <v>1.501</v>
       </c>
       <c r="D69" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D69+0.001</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="E69" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K69</f>
-        <v>101.25</v>
+        <v>125.8</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28946,15 +28901,15 @@
       </c>
       <c r="C70" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C70=0,0,'Rate definitions 2'!C70+0.001)</f>
-        <v>1.501</v>
+        <v>2.001</v>
       </c>
       <c r="D70" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D70+0.001</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="E70" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K70</f>
-        <v>125.8</v>
+        <v>158.5</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28968,43 +28923,21 @@
       </c>
       <c r="C71" s="0" t="n">
         <f aca="false">IF('Rate definitions 2'!C71=0,0,'Rate definitions 2'!C71+0.001)</f>
-        <v>2.001</v>
+        <v>3.001</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">'Rate definitions 2'!D71+0.001</f>
-        <v>3.001</v>
+        <v>5.001</v>
       </c>
       <c r="E71" s="6" t="n">
         <f aca="false">'Rate definitions 2'!K71</f>
-        <v>158.5</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="str">
-        <f aca="false">VLOOKUP('Rate definitions 2'!A72,Lookup!$A$3:$B$12,2,FALSE())</f>
-        <v>Zone 9: Rest of World 2</v>
-      </c>
-      <c r="B72" s="0" t="str">
-        <f aca="false">'Rate definitions 2'!F72</f>
-        <v>International Insured Express</v>
-      </c>
-      <c r="C72" s="0" t="n">
-        <f aca="false">IF('Rate definitions 2'!C72=0,0,'Rate definitions 2'!C72+0.001)</f>
-        <v>3.001</v>
-      </c>
-      <c r="D72" s="0" t="n">
-        <f aca="false">'Rate definitions 2'!D72+0.001</f>
-        <v>5.001</v>
-      </c>
-      <c r="E72" s="6" t="n">
-        <f aca="false">'Rate definitions 2'!K72</f>
         <v>223.9</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -29019,11 +28952,11 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -29067,7 +29000,7 @@
         <v>1611</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1650</v>
+        <v>607</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29083,7 +29016,7 @@
         <v>1613</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>1651</v>
+        <v>950</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29113,7 +29046,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>